<commit_message>
Now templates are easy to pre-fill with custom data.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.1.xlsx
+++ b/schema_definitions/template_schema_v1.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F2BE98-0CC6-5A49-884C-6C0F4E66B7A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FEF65E-43CB-7342-83F6-17EA03878310}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
@@ -980,7 +980,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Small bits, improved documentation.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.1.xlsx
+++ b/schema_definitions/template_schema_v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FEF65E-43CB-7342-83F6-17EA03878310}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2E34D8-8E4C-EB43-A6EC-E6C6ED1B60C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="33960" yWindow="-4160" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="notes" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">association!$C$1:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">association!$C$1:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">study!$C$1:$C$18</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -979,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -987,7 +987,7 @@
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" customWidth="1"/>
@@ -1463,11 +1463,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1548,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>153</v>
       </c>
@@ -1664,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>141</v>
       </c>
@@ -1774,7 +1773,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>128</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>127</v>
       </c>
       <c r="C11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>0</v>
@@ -1800,15 +1799,15 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>0</v>
@@ -1821,46 +1820,46 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="b">
         <v>0</v>
@@ -1873,38 +1872,38 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>114</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>113</v>
       </c>
       <c r="C16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="b">
         <v>0</v>
@@ -1931,13 +1930,7 @@
       <c r="L16" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C16" xr:uid="{692A23DE-1971-9644-BCB5-0858E868D84D}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C16" xr:uid="{692A23DE-1971-9644-BCB5-0858E868D84D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>